<commit_message>
Update data for parser defects
</commit_message>
<xml_diff>
--- a/processed_data/_2018-2019.xlsx
+++ b/processed_data/_2018-2019.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1920" yWindow="730" windowWidth="23200" windowHeight="13750" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1920" yWindow="732" windowWidth="23196" windowHeight="13176" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Summer 2018" sheetId="1" state="visible" r:id="rId1"/>
@@ -21,14 +21,14 @@
   <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <family val="3"/>
       <sz val="9"/>
@@ -59,7 +59,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -388,7 +388,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -402,27 +402,27 @@
   </sheetPr>
   <dimension ref="A1:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="R52" sqref="R52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
-    <col width="7.453125" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="9.26953125" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="33.453125" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="13.54296875" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="10.90625" bestFit="1" customWidth="1" min="5" max="5"/>
-    <col width="21.453125" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="17.90625" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="12.08984375" bestFit="1" customWidth="1" min="8" max="8"/>
+    <col width="7.44140625" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="9.21875" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="33.44140625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="13.5546875" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="10.88671875" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="21.44140625" bestFit="1" customWidth="1" min="6" max="6"/>
+    <col width="17.88671875" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="12.109375" bestFit="1" customWidth="1" min="8" max="8"/>
     <col width="12" bestFit="1" customWidth="1" min="9" max="10"/>
-    <col width="12.1796875" bestFit="1" customWidth="1" min="11" max="11"/>
-    <col width="11.81640625" bestFit="1" customWidth="1" min="12" max="12"/>
-    <col width="11.90625" bestFit="1" customWidth="1" min="13" max="13"/>
-    <col width="13.26953125" bestFit="1" customWidth="1" min="14" max="14"/>
-    <col width="7.26953125" bestFit="1" customWidth="1" min="15" max="15"/>
-    <col width="9.1796875" bestFit="1" customWidth="1" min="16" max="16"/>
+    <col width="12.21875" bestFit="1" customWidth="1" min="11" max="11"/>
+    <col width="11.77734375" bestFit="1" customWidth="1" min="12" max="12"/>
+    <col width="11.88671875" bestFit="1" customWidth="1" min="13" max="13"/>
+    <col width="13.21875" bestFit="1" customWidth="1" min="14" max="14"/>
+    <col width="7.21875" bestFit="1" customWidth="1" min="15" max="15"/>
+    <col width="9.21875" bestFit="1" customWidth="1" min="16" max="16"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1261,7 +1261,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>POLICY  TEACHING</t>
+          <t>POLICY &amp; TEACHING</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1327,7 +1327,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>POLICY  TEACHING</t>
+          <t>POLICY &amp; TEACHING</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1393,7 +1393,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>POLICY  TEACHING</t>
+          <t>POLICY &amp; TEACHING</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1459,7 +1459,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>POLICY  TEACHING</t>
+          <t>POLICY &amp; TEACHING</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1525,7 +1525,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>LRN IN SCHL</t>
+          <t>LRN IN&amp;OUT SCHL</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1591,7 +1591,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>LRN IN SCHL</t>
+          <t>LRN IN&amp;OUT SCHL</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -2581,7 +2581,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>LEARNG  CHILD DEV</t>
+          <t>LEARNG &amp; CHILD DEV</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -3637,7 +3637,7 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>FN:TRADE  MKTMICRO</t>
+          <t>FN:TRADE &amp; MKTMICRO</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
@@ -4217,23 +4217,23 @@
   </sheetPr>
   <dimension ref="A1:P341"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R335" sqref="R335"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
-    <col width="8.54296875" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="9.54296875" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="32.6328125" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="15.453125" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="11.6328125" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="8.5546875" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="9.5546875" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="32.6640625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="15.44140625" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="11.6640625" bestFit="1" customWidth="1" min="5" max="5"/>
     <col width="24" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="63.453125" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="12.81640625" bestFit="1" customWidth="1" min="8" max="13"/>
-    <col width="13.90625" bestFit="1" customWidth="1" min="14" max="14"/>
-    <col width="7.54296875" bestFit="1" customWidth="1" min="15" max="15"/>
-    <col width="10.54296875" bestFit="1" customWidth="1" min="16" max="16"/>
+    <col width="63.44140625" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="12.77734375" bestFit="1" customWidth="1" min="8" max="13"/>
+    <col width="13.88671875" bestFit="1" customWidth="1" min="14" max="14"/>
+    <col width="7.5546875" bestFit="1" customWidth="1" min="15" max="15"/>
+    <col width="10.5546875" bestFit="1" customWidth="1" min="16" max="16"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -9362,7 +9362,7 @@
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>DEV &amp; CELL JRNL CLUB</t>
+          <t>DEV &amp;CELL JRNL CLUB</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
@@ -11540,7 +11540,7 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>RES EPISTEMOL &amp; METH</t>
+          <t>RES EPISTEMOL &amp;METH</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
@@ -14180,7 +14180,7 @@
       </c>
       <c r="F151" t="inlineStr">
         <is>
-          <t>SENS ACTU &amp; SENS NET</t>
+          <t>SENS ACTU &amp;SENS NET</t>
         </is>
       </c>
       <c r="G151" t="inlineStr">
@@ -18206,7 +18206,7 @@
       </c>
       <c r="F212" t="inlineStr">
         <is>
-          <t>BLCKCHAN &amp; CRYPTOCUR</t>
+          <t>BLCKCHAN &amp;CRYPTOCUR</t>
         </is>
       </c>
       <c r="G212" t="inlineStr">
@@ -24674,7 +24674,7 @@
       </c>
       <c r="F310" t="inlineStr">
         <is>
-          <t>INFO &amp; PUBLIC POLICY</t>
+          <t>INFO &amp;PUBLIC POLICY</t>
         </is>
       </c>
       <c r="G310" t="inlineStr">
@@ -26772,23 +26772,23 @@
   </sheetPr>
   <dimension ref="A1:P303"/>
   <sheetViews>
-    <sheetView topLeftCell="A279" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G189" sqref="G189"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R300" sqref="R300"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
-    <col width="8.54296875" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="9.54296875" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="32.6328125" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="13.90625" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="11.6328125" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="8.5546875" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="9.5546875" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="32.6640625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="13.88671875" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="11.6640625" bestFit="1" customWidth="1" min="5" max="5"/>
     <col width="24" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="48.81640625" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="12.81640625" bestFit="1" customWidth="1" min="8" max="13"/>
-    <col width="13.90625" bestFit="1" customWidth="1" min="14" max="14"/>
-    <col width="7.54296875" bestFit="1" customWidth="1" min="15" max="15"/>
-    <col width="10.54296875" bestFit="1" customWidth="1" min="16" max="16"/>
+    <col width="48.77734375" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="12.77734375" bestFit="1" customWidth="1" min="8" max="13"/>
+    <col width="13.88671875" bestFit="1" customWidth="1" min="14" max="14"/>
+    <col width="7.5546875" bestFit="1" customWidth="1" min="15" max="15"/>
+    <col width="10.5546875" bestFit="1" customWidth="1" min="16" max="16"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -31455,7 +31455,7 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>DEV &amp; CELL JRNL CLUB</t>
+          <t>DEV &amp;CELL JRNL CLUB</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
@@ -40101,7 +40101,7 @@
       </c>
       <c r="F202" t="inlineStr">
         <is>
-          <t>ACCTNG POLICY &amp; RSCH</t>
+          <t>ACCTNG POLICY &amp;RSCH</t>
         </is>
       </c>
       <c r="G202" t="inlineStr">
@@ -46819,23 +46819,23 @@
   </sheetPr>
   <dimension ref="A1:P281"/>
   <sheetViews>
-    <sheetView topLeftCell="A259" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G200" sqref="G200"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4" outlineLevelCol="0"/>
   <cols>
-    <col width="8.54296875" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="9.54296875" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="32.6328125" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="13.90625" bestFit="1" customWidth="1" min="4" max="4"/>
-    <col width="11.6328125" bestFit="1" customWidth="1" min="5" max="5"/>
+    <col width="8.5546875" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="9.5546875" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="32.6640625" bestFit="1" customWidth="1" min="3" max="3"/>
+    <col width="13.88671875" bestFit="1" customWidth="1" min="4" max="4"/>
+    <col width="11.6640625" bestFit="1" customWidth="1" min="5" max="5"/>
     <col width="24" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="53.54296875" bestFit="1" customWidth="1" min="7" max="7"/>
-    <col width="12.81640625" bestFit="1" customWidth="1" min="8" max="13"/>
-    <col width="13.90625" bestFit="1" customWidth="1" min="14" max="14"/>
-    <col width="7.54296875" bestFit="1" customWidth="1" min="15" max="15"/>
-    <col width="10.54296875" bestFit="1" customWidth="1" min="16" max="16"/>
+    <col width="53.5546875" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="12.77734375" bestFit="1" customWidth="1" min="8" max="13"/>
+    <col width="13.88671875" bestFit="1" customWidth="1" min="14" max="14"/>
+    <col width="7.5546875" bestFit="1" customWidth="1" min="15" max="15"/>
+    <col width="10.5546875" bestFit="1" customWidth="1" min="16" max="16"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -49456,7 +49456,7 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>MERGING MODLS &amp; DATA</t>
+          <t>MERGING MODLS &amp;DATA</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -56980,7 +56980,7 @@
       </c>
       <c r="F154" t="inlineStr">
         <is>
-          <t>FE:EDGE</t>
+          <t>FE: EDGE</t>
         </is>
       </c>
       <c r="G154" t="inlineStr">
@@ -59488,7 +59488,7 @@
       </c>
       <c r="F192" t="inlineStr">
         <is>
-          <t>FN:VEN CAP &amp; PRIV EQ</t>
+          <t>FN:VEN CAP &amp;PRIV EQ</t>
         </is>
       </c>
       <c r="G192" t="inlineStr">
@@ -60148,7 +60148,7 @@
       </c>
       <c r="F202" t="inlineStr">
         <is>
-          <t>ACCTG INCOME TAX</t>
+          <t>ACCTG  INCOME TAX</t>
         </is>
       </c>
       <c r="G202" t="inlineStr">

</xml_diff>